<commit_message>
add hash to save datafiles
</commit_message>
<xml_diff>
--- a/12_08_txtToXlsx/saveTable.xlsx
+++ b/12_08_txtToXlsx/saveTable.xlsx
@@ -16,64 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>AAAAAA</t>
-  </si>
-  <si>
-    <t>BBBBBB</t>
-  </si>
-  <si>
-    <t>CCCCCC</t>
-  </si>
-  <si>
-    <t>DDDDDD</t>
-  </si>
-  <si>
-    <t>This my manifest</t>
-  </si>
-  <si>
-    <t>Hello</t>
-  </si>
-  <si>
-    <t>HelloHello</t>
-  </si>
-  <si>
-    <t>HelloHelloHello</t>
-  </si>
-  <si>
-    <t>HelloHelloHelloHello</t>
-  </si>
-  <si>
-    <t>HelloHelloHelloHelloHello</t>
-  </si>
-  <si>
-    <t>HelloHelloHelloHelloHelloHello</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
-    <font>
-      <sz val="12"/>
-      <name val="Verdana"/>
-      <family val="0"/>
-      <charset val="0"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="00000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-  </fills>
   <borders count="1">
     <border>
       <left style="none"/>
@@ -82,10 +29,7 @@
       <bottom style="none"/>
     </border>
   </borders>
-  <cellXfs count="2">
-    <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
-    </xf>
+  <cellXfs count="1">
     <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -418,73 +362,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.5"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
+  <cols/>
+  <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>